<commit_message>
this is my intitial commit
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/TestData.xlsx
+++ b/src/test/resources/configs/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clintonr\Documents\Salesforce.Automation\src\test\resources\configs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RamsundarSP\Salesforce.Automation\src\test\resources\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FCD1FB-1BDB-4E3F-81D7-58247F1D07EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C93FA13-7098-4939-B18A-57DAEEB8ED7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application_Config" sheetId="4" r:id="rId1"/>
@@ -210,18 +210,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -571,47 +566,47 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -662,25 +657,25 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="3"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.1796875" style="3"/>
+    <col min="17" max="17" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -696,82 +691,82 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="7">
         <v>2</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="5" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="7">
         <v>3</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>